<commit_message>
fix(reader): datetime parsing adjustment
datetime of value 0 is parsed correctly as 0:00 now
</commit_message>
<xml_diff>
--- a/src/test/resources/workbook-1904.xlsx
+++ b/src/test/resources/workbook-1904.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\WorkbookEventReader\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BCB699-D255-435D-B1F5-F0E1D23441D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D421060-D5CB-4259-82F0-ED09D93469C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1185" windowWidth="18945" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9330" yWindow="2085" windowWidth="18945" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +201,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -224,7 +232,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -259,6 +267,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -539,7 +550,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -601,6 +612,9 @@
       </c>
       <c r="C3" s="7">
         <v>0.89584490740740697</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>